<commit_message>
Added video and some modifications
</commit_message>
<xml_diff>
--- a/FinalRecords.xlsx
+++ b/FinalRecords.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,55 +436,55 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Samsung Galaxy M32 5G (Sky Blue, 8GB RAM, 128GB Storage)</t>
+          <t>Samsung Galaxy M32 5G (Sky Blue, 6GB RAM, 128GB Storage)</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>18,999</t>
+          <t>16,999</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Samsung Galaxy M31 (Ocean Blue, 8GB RAM, 128GB Storage) 6 Months Free Screen Replacement for Prime</t>
+          <t>Samsung Galaxy Note 20 (Mystic Green, 8GB RAM, 256GB Storage) with No Cost EMI/Additional Exchange Offers</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>15,999</t>
+          <t>44,999</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Samsung Galaxy M12 (Blue,4GB RAM, 64GB Storage) 6000 mAh with 8nm Processor | True 48 MP Quad Camera | 90Hz Refresh Rate</t>
+          <t>Samsung Galaxy M32 5G (Sky Blue, 8GB RAM, 128GB Storage)</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>9,499</t>
+          <t>18,999</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Samsung Galaxy M12 (Black,6GB RAM, 128GB Storage) 6 Months Free Screen Replacement for Prime</t>
+          <t>Samsung Galaxy M31 (Ocean Blue, 8GB RAM, 128GB Storage) 6 Months Free Screen Replacement for Prime</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>11,499</t>
+          <t>15,999</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Samsung Galaxy M32 5G (Sky Blue, 8GB RAM, 128GB Storage)</t>
+          <t>Samsung Galaxy M32 5G (Slate Black, 8GB RAM, 128GB Storage)</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -496,187 +496,187 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Samsung Galaxy M32 (Black, 4GB RAM, 64GB Storage) 6 Months Free Screen Replacement for Prime</t>
+          <t>Samsung Galaxy M32 (Light Blue, 6GB RAM, 128GB Storage) 6 Months Free Screen Replacement for Prime</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>12,999</t>
+          <t>14,999</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Samsung Galaxy M21 2021 Edition (Arctic Blue, 4GB RAM, 64GB Storage) | FHD+ sAMOLED | 6 Months Free Screen Replacement for Prime (SM-M215GLBDINS)</t>
+          <t>Samsung Galaxy M32 (Black, 4GB RAM, 64GB Storage) 6 Months Free Screen Replacement for Prime</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>11,999</t>
+          <t>12,999</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Samsung Galaxy M32 (Black, 6GB RAM, 128GB Storage) 6 Months Free Screen Replacement for Prime</t>
+          <t>Samsung Galaxy M12 (Blue,4GB RAM, 64GB Storage) 6000 mAh with 8nm Processor | True 48 MP Quad Camera | 90Hz Refresh Rate</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>14,999</t>
+          <t>9,499</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Samsung Galaxy M12 (Black,4GB RAM, 64GB Storage) 6000 mAh with 8nm Processor | True 48 MP Quad Camera | 90Hz Refresh Rate</t>
+          <t>Samsung Galaxy M21 2021 Edition (Arctic Blue, 4GB RAM, 64GB Storage) | FHD+ sAMOLED | 6 Months Free Screen Replacement for Prime (SM-M215GLBDINS)</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>9,499</t>
+          <t>11,999</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Samsung Galaxy M12 (Blue,6GB RAM, 128GB Storage) 6 Months Free Screen Replacement for Prime</t>
+          <t>Samsung Galaxy M51 (Celestial Black, 6GB RAM, 128GB Storage) 6 Months Free Screen Replacement for Prime</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>11,499</t>
+          <t>19,999</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Samsung Galaxy M32 5G (Slate Black, 8GB RAM, 128GB Storage)</t>
+          <t>Samsung Galaxy M32 5G (Sky Blue, 6GB RAM, 128GB Storage)</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>18,999</t>
+          <t>16,999</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Samsung Galaxy M51 (Celestial Black, 6GB RAM, 128GB Storage) 6 Months Free Screen Replacement for Prime</t>
+          <t>Samsung Galaxy M12 (Black,6GB RAM, 128GB Storage) 6 Months Free Screen Replacement for Prime</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>19,999</t>
+          <t>11,499</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Samsung Galaxy M32 (Light Blue, 6GB RAM, 128GB Storage) 6 Months Free Screen Replacement for Prime</t>
+          <t>Samsung Galaxy M12 (Black,4GB RAM, 64GB Storage) 6000 mAh with 8nm Processor | True 48 MP Quad Camera | 90Hz Refresh Rate</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>14,999</t>
+          <t>9,499</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Samsung Galaxy Note 20 (Mystic Green, 8GB RAM, 256GB Storage) with No Cost EMI/Additional Exchange Offers</t>
+          <t>Samsung Galaxy M32 (Light Blue, 4GB RAM, 64GB Storage) 6 Months Free Screen Replacement for Prime</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>44,990</t>
+          <t>12,999</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Samsung Guru Music 2 (SM-B310E, Blue)</t>
+          <t>Samsung Galaxy M32 (Black, 6GB RAM, 128GB Storage) 6 Months Free Screen Replacement for Prime</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2,350</t>
+          <t>14,999</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Samsung Galaxy M32 5G (Sky Blue, 6GB RAM, 128GB Storage)</t>
+          <t>Samsung Galaxy M52 5G (Blazing Black, 6GB RAM, 128GB Storage) Latest Snapdragon 778G 5G | sAMOLED 120Hz Display</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>16,999</t>
+          <t>25,999</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Samsung Galaxy M32 5G (Slate Black, 6GB RAM, 128GB Storage)</t>
+          <t>Samsung Galaxy M12 (Blue,6GB RAM, 128GB Storage) 6 Months Free Screen Replacement for Prime</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>16,999</t>
+          <t>11,499</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Samsung Galaxy M21 2021 Edition (Charcoal Black, 4GB RAM, 64GB Storage) | FHD+ sAMOLED | 6 Months Free Screen Replacement for Prime (SM-M215GZKDINS)</t>
+          <t>Samsung Galaxy M12 (White,6GB RAM, 128GB Storage) 6 Months Free Screen Replacement for Prime</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>11,999</t>
+          <t>11,499</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Samsung Galaxy M52 5G (Blazing Black, 6GB RAM, 128GB Storage) Latest Snapdragon 778G 5G | sAMOLED 120Hz Display</t>
+          <t>Samsung Galaxy S20 FE 5G (Cloud Navy, 8GB RAM, 128GB Storage)</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>25,999</t>
+          <t>36,990</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Samsung Galaxy M12 (White,6GB RAM, 128GB Storage) 6 Months Free Screen Replacement for Prime</t>
+          <t>Samsung Galaxy M21 2021 Edition (Charcoal Black, 4GB RAM, 64GB Storage) | FHD+ sAMOLED | 6 Months Free Screen Replacement for Prime (SM-M215GZKDINS)</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>11,499</t>
+          <t>11,999</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Samsung Guru 1200 (GT-E1200, Black)</t>
+          <t>Samsung Galaxy M21 2021 Edition (Arctic Blue, 6GB RAM, 128GB Storage) | FHD+ sAMOLED | 6 Months Free Screen Replacement for Prime (SM-M215GLBHINS)</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -688,7 +688,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Samsung Galaxy M21 2021 Edition (Arctic Blue, 6GB RAM, 128GB Storage) | FHD+ sAMOLED | 6 Months Free Screen Replacement for Prime (SM-M215GLBHINS)</t>
+          <t>Samsung Galaxy M31 (Space Black, 8GB RAM, 128GB Storage) 6 Months Free Screen Replacement for Prime</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -700,24 +700,48 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Samsung Galaxy M31 (Space Black, 8GB RAM, 128GB Storage) 6 Months Free Screen Replacement for Prime</t>
+          <t>Samsung Galaxy M52 5G (Blazing Black, 8GB RAM, 128GB Storage) Latest Snapdragon 778G 5G | sAMOLED 120Hz Display</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>13,999</t>
+          <t>27,999</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Samsung Galaxy M21 2021 Edition (Charcoal black, 6GB RAM, 128GB Storage) | FHD+ sAMOLED | 6 Months Free Screen Replacement for Prime (SM-M215GZKHINS)</t>
+          <t>Samsung Galaxy M51 (Electric Blue, 6GB RAM, 128GB Storage) 6 Months Free Screen Replacement for Prime</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>21,998</t>
+          <t>19,999</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Samsung Galaxy A22 (Black, 6GB RAM, 128GB Storage) with No Cost EMI/Additional Exchange Offers</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>18,499</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Samsung Galaxy M52 5G (ICY Blue, 6GB RAM, 128GB Storage) Latest Snapdragon 778G 5G | sAMOLED 120Hz Display</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>25,999</t>
         </is>
       </c>
     </row>

</xml_diff>